<commit_message>
Replace text in spreadsheet
</commit_message>
<xml_diff>
--- a/assets/demo.xlsx
+++ b/assets/demo.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <fileSharing readOnlyRecommended="0" userName="gabri"/>
+  <fileSharing readOnlyRecommended="0" userName="gabriel"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId4"/>
@@ -14,10 +14,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1565786227" val="966" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1565786227" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1565786227" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1565786227"/>
+      <pm:revision xmlns:pm="smNativeData" day="1646843021" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1646843021" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1646843021" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1646843021"/>
     </ext>
   </extLst>
 </workbook>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>modelo</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>D1</t>
+  </si>
+  <si>
+    <t>{tag}</t>
   </si>
   <si>
     <t xml:space="preserve">Resperado = </t>
@@ -260,17 +263,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
-    <numFmt numFmtId="5" formatCode="#,##0\ &quot;R$&quot;;\-#,##0\ &quot;R$&quot;"/>
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;R$&quot;;[Red]\-#,##0\ &quot;R$&quot;"/>
-    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;R$&quot;;\-#,##0.00\ &quot;R$&quot;"/>
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;R$&quot;;[Red]\-#,##0.00\ &quot;R$&quot;"/>
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;R$&quot;_-;\-* #,##0\ &quot;R$&quot;_-;_-* &quot;-&quot;\ &quot;R$&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0\ _R_$_-;\-* #,##0\ _R_$_-;_-* &quot;-&quot;\ _R_$_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;R$&quot;_-;\-* #,##0.00\ &quot;R$&quot;_-;_-* &quot;-&quot;??\ &quot;R$&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _R_$_-;\-* #,##0.00\ _R_$_-;_-* &quot;-&quot;??\ _R_$_-;_-@_-"/>
+    <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
+    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;$&quot;;[Red]\-#,##0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;$&quot;_-;\-* #,##0\ &quot;$&quot;_-;_-* &quot;-&quot;\ &quot;$&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0\ _$_-;\-* #,##0\ _$_-;_-* &quot;-&quot;\ _$_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="DD/MM"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -278,10 +281,25 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1565786227" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646843021" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Basic Sans"/>
+      <family val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646843021" ulstyle="none" kern="1">
+            <pm:latin face="Basic Sans" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -293,7 +311,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1565786227" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1646843021" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="240" lang="default"/>
             <pm:cs face="Times New Roman" sz="240" lang="default"/>
             <pm:ea face="SimSun" sz="240" lang="default"/>
@@ -302,7 +320,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,7 +336,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1565786227" type="1" fgLvl="38" fgClr="000000FF" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1646843021" type="1" fgLvl="38" fgClr="000000FF" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -377,7 +395,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1565786227" type="1" fgLvl="38" fgClr="0000FFFF" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1646843021" type="1" fgLvl="38" fgClr="0000FFFF" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -388,7 +406,18 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1565786227" type="1" fgLvl="38" fgClr="0000FFFF" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1646843021" type="1" fgLvl="38" fgClr="0000FFFF" bgLvl="62" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5C5C"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1646843021" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -399,35 +428,13 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1565786227" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9EFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1565786227" type="1" fgLvl="38" fgClr="0000FFFF" bgLvl="62" bgClr="00FFFFFF"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF5C5C"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1565786227" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1646843021" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -443,7 +450,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227"/>
+          <pm:border xmlns:pm="smNativeData" id="1646843021"/>
         </ext>
       </extLst>
     </border>
@@ -462,7 +469,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -486,7 +493,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227"/>
+          <pm:border xmlns:pm="smNativeData" id="1646843021"/>
         </ext>
       </extLst>
     </border>
@@ -505,7 +512,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -529,7 +536,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -552,7 +559,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -575,7 +582,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -599,7 +606,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -620,7 +627,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -641,7 +648,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -662,7 +669,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -684,7 +691,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -705,7 +712,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -727,7 +734,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -748,7 +755,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -769,7 +776,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -791,7 +798,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="bottom" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -813,7 +820,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -836,7 +843,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -858,7 +865,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -880,7 +887,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227">
+          <pm:border xmlns:pm="smNativeData" id="1646843021">
             <pm:line position="top" type="1" style="0" width="40" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -903,7 +910,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227"/>
+          <pm:border xmlns:pm="smNativeData" id="1646843021"/>
         </ext>
       </extLst>
     </border>
@@ -922,26 +929,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1565786227"/>
+          <pm:border xmlns:pm="smNativeData" id="1646843021"/>
         </ext>
       </extLst>
     </border>
@@ -954,64 +942,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1020,7 +1008,7 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="23" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="21" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1030,12 +1018,13 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1565786227" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1646843021" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1565786227" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1646843021" count="3">
         <pm:color name="Cor 24" rgb="9E9EFF"/>
         <pm:color name="Cor 25" rgb="9EFFFF"/>
+        <pm:color name="Color 26" rgb="FF5C5C"/>
       </pm:colors>
     </ext>
   </extLst>
@@ -1047,10 +1036,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="D5D5D5"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="494949"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="EEECE1"/>
@@ -1300,11 +1289,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView view="normal" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
   <cols>
     <col min="1" max="1" width="13.702703" customWidth="1" style="1"/>
     <col min="2" max="3" width="14.567568" customWidth="1" style="1"/>
@@ -1549,12 +1538,15 @@
         <v>8.30610633950599997</v>
       </c>
     </row>
-    <row r="12" spans="3:5">
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E12" s="4"/>
     </row>
@@ -1572,7 +1564,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1565786227" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1646843021" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1581,16 +1573,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1565786227" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1565786227" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1565786227" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1565786227" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1646843021" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1646843021" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1565786227" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1646843021" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1603,11 +1593,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
   <cols>
     <col min="1" max="1" width="10.000000" style="1"/>
     <col min="2" max="2" width="11.117117" customWidth="1" style="1"/>
@@ -1622,7 +1612,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="n">
         <v>10</v>
@@ -1699,30 +1689,30 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>6.12999999999999989</v>
@@ -1748,7 +1738,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>6.19000000000000039</v>
@@ -1774,7 +1764,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>6.21999999999999975</v>
@@ -1800,7 +1790,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>6.29000000000000004</v>
@@ -1826,7 +1816,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>6.20000000000000018</v>
@@ -1852,7 +1842,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>6.25</v>
@@ -1878,7 +1868,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>6.17999999999999972</v>
@@ -1904,7 +1894,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="9" t="n">
         <v>5.99000000000000021</v>
@@ -1930,7 +1920,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>8.33000000000000007</v>
@@ -1956,7 +1946,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>8.33000000000000007</v>
@@ -1982,7 +1972,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>8.34999999999999787</v>
@@ -2017,30 +2007,30 @@
         <v>2</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>8.5</v>
@@ -2078,7 +2068,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>6.33999999999999986</v>
@@ -2116,7 +2106,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>6.07000000000000028</v>
@@ -2154,7 +2144,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>5.84999999999999964</v>
@@ -2192,7 +2182,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>5.88999999999999968</v>
@@ -2230,7 +2220,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>5.92999999999999972</v>
@@ -2268,7 +2258,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>5.87999999999999989</v>
@@ -2306,7 +2296,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>5.59999999999999964</v>
@@ -2344,7 +2334,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>5.63999999999999968</v>
@@ -2382,7 +2372,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>5.75999999999999979</v>
@@ -2420,7 +2410,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>6.00999999999999979</v>
@@ -2458,7 +2448,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>5.94000000000000039</v>
@@ -2496,7 +2486,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>5.98000000000000043</v>
@@ -2534,7 +2524,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>6.04999999999999982</v>
@@ -2572,7 +2562,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>6.30999999999999961</v>
@@ -2610,7 +2600,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>5.95999999999999996</v>
@@ -2648,7 +2638,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>6.25999999999999979</v>
@@ -2686,7 +2676,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>6.26999999999999957</v>
@@ -2724,7 +2714,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>6.29000000000000004</v>
@@ -2762,7 +2752,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>6.58000000000000007</v>
@@ -2800,7 +2790,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>6.67999999999999972</v>
@@ -2838,7 +2828,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>6.90000000000000036</v>
@@ -2876,7 +2866,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>6.95999999999999996</v>
@@ -2914,7 +2904,7 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>6.29999999999999982</v>
@@ -2952,7 +2942,7 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>6.11000000000000032</v>
@@ -2990,7 +2980,7 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>5.59999999999999964</v>
@@ -3028,7 +3018,7 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B51" s="9" t="n">
         <v>5.83000000000000007</v>
@@ -3069,7 +3059,7 @@
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
       <c r="D52" s="22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E52" s="22">
         <f>AVERAGE(E25:E51)</f>
@@ -3098,7 +3088,7 @@
     </row>
     <row r="53" spans="4:10">
       <c r="D53" s="24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E53" s="24">
         <f>MAX(E25:E52)</f>
@@ -3129,7 +3119,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1565786227" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1646843021" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3138,17 +3128,15 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1565786227" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1565786227" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1565786227" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1565786227" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1646843021" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1646843021" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1565786227" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1646843021" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>